<commit_message>
Clean unused old code for activation times
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20343"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP_TB_BMC_MED\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D437E41F-6B19-4ED5-99B4-C00051229A8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97BD0F-1658-446B-887A-0934AF2DDBD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="239">
   <si>
     <t>project_name</t>
   </si>
@@ -136,9 +136,6 @@
     <t>force_tb_init</t>
   </si>
   <si>
-    <t>generate_activation_times</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -742,13 +739,10 @@
     <t>prevalence_by_age_record_time</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>for_analysis</t>
   </si>
   <si>
-    <t>analysis_14_05</t>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,17 +1161,17 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,17 +1179,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1239,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1253,7 +1247,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
@@ -1288,46 +1282,44 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>238</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>1</v>
@@ -1335,35 +1327,35 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="6"/>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
@@ -1372,7 +1364,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>0</v>
@@ -1384,7 +1376,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>0</v>
@@ -1395,20 +1387,20 @@
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3"/>
+      <c r="A19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B20" s="7" t="b">
         <v>1</v>
@@ -1420,7 +1412,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" s="7" t="b">
         <v>1</v>
@@ -1432,10 +1424,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>22</v>
+        <v>207</v>
       </c>
       <c r="B22" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>10</v>
@@ -1456,10 +1448,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>209</v>
+        <v>23</v>
       </c>
       <c r="B24" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>10</v>
@@ -1468,19 +1460,21 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26" s="7" t="b">
         <v>0</v>
@@ -1494,7 +1488,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="7" t="b">
         <v>0</v>
@@ -1502,13 +1496,11 @@
       <c r="C27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="7" t="b">
         <v>0</v>
@@ -1520,10 +1512,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>28</v>
+        <v>197</v>
       </c>
       <c r="B29" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>10</v>
@@ -1532,7 +1524,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B30" s="7" t="b">
         <v>1</v>
@@ -1540,11 +1532,13 @@
       <c r="C30" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="D30" s="7" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B31" s="7" t="b">
         <v>1</v>
@@ -1552,13 +1546,11 @@
       <c r="C31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>205</v>
-      </c>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>202</v>
+        <v>231</v>
       </c>
       <c r="B32" s="7" t="b">
         <v>1</v>
@@ -1569,46 +1561,46 @@
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="B33" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="7"/>
+      <c r="A33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="6" t="b">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="B34" s="6">
+        <v>50</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="6">
-        <v>50</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>32</v>
+      <c r="A35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>33</v>
+        <v>222</v>
       </c>
       <c r="B36" s="5" t="b">
         <v>1</v>
@@ -1616,56 +1608,55 @@
       <c r="C36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="6"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B37" s="5" t="b">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="b">
         <v>1</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="5"/>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" t="b">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
+      <c r="A38" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="8" t="b">
+      <c r="A39" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" t="b">
         <v>0</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B41" t="b">
         <v>0</v>
@@ -1676,146 +1667,146 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>201</v>
-      </c>
-      <c r="B42" t="b">
-        <v>0</v>
+        <v>198</v>
+      </c>
+      <c r="B42">
+        <v>2000</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="D42" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="12"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" s="11">
+        <v>50</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="B43">
-        <v>2000</v>
-      </c>
-      <c r="C43" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D44" s="12"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="B45" s="11">
-        <v>50</v>
+        <v>202</v>
+      </c>
+      <c r="B45" s="11" t="b">
+        <v>0</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>200</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B46" s="11" t="b">
+      <c r="A46" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B46" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="11"/>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B47" s="2" t="b">
-        <v>0</v>
+      <c r="B47" s="2">
+        <v>100</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B48" s="2">
-        <v>100</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>7</v>
+      <c r="A48" t="s">
+        <v>226</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>227</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>230</v>
+        <v>213</v>
+      </c>
+      <c r="B49">
+        <v>1920</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>214</v>
-      </c>
-      <c r="B50">
-        <v>1920</v>
+        <v>220</v>
+      </c>
+      <c r="B50" t="s">
+        <v>215</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" t="s">
-        <v>216</v>
+        <v>230</v>
+      </c>
+      <c r="B51">
+        <v>2018</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>231</v>
-      </c>
-      <c r="B52">
-        <v>2018</v>
+        <v>233</v>
+      </c>
+      <c r="B52" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>234</v>
-      </c>
-      <c r="B53" s="6" t="b">
-        <v>1</v>
+        <v>235</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1823,26 +1814,15 @@
         <v>236</v>
       </c>
       <c r="B54">
-        <v>5</v>
+        <v>2010</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>237</v>
-      </c>
-      <c r="B55">
-        <v>2010</v>
-      </c>
-      <c r="C55" s="11" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -1856,37 +1836,37 @@
           <x14:formula1>
             <xm:f>dropdown!$A$1:$B$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B53 B36:B39 B8:B11 B15:B34</xm:sqref>
+          <xm:sqref>B52 B35:B38 B8:B10 B14:B33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>dropdown!$E$1:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B14</xm:sqref>
+          <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>dropdown!$G$1:$G$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B40</xm:sqref>
+          <xm:sqref>B39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>dropdown!$K$1:$K$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B44</xm:sqref>
+          <xm:sqref>B43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>dropdown!$I$9:$I$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B51</xm:sqref>
+          <xm:sqref>B50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>dropdown!$G$6:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B49</xm:sqref>
+          <xm:sqref>B48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1920,830 +1900,830 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" t="s">
         <v>217</v>
-      </c>
-      <c r="K3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean unused parameters from console.xlsx
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97BD0F-1658-446B-887A-0934AF2DDBD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722BDA67-658F-4C4A-AD1D-B0802D88B560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="234">
   <si>
     <t>project_name</t>
   </si>
@@ -643,12 +643,6 @@
     <t>/1000pop/y</t>
   </si>
   <si>
-    <t>freeze_demo</t>
-  </si>
-  <si>
-    <t>time_demo_freezing</t>
-  </si>
-  <si>
     <t>plot_ts_tb_prevalence_ds</t>
   </si>
   <si>
@@ -658,9 +652,6 @@
     <t>find_a_calibrated_model</t>
   </si>
   <si>
-    <t>calibration_tolerance</t>
-  </si>
-  <si>
     <t>run_ks_based_calibration</t>
   </si>
   <si>
@@ -698,12 +689,6 @@
   </si>
   <si>
     <t>run_full_calibration</t>
-  </si>
-  <si>
-    <t>Find_calibrated_model</t>
-  </si>
-  <si>
-    <t>Final_simulation</t>
   </si>
   <si>
     <t>fixed_birth_rate_based_on</t>
@@ -1145,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1141,7 @@
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1171,7 +1156,7 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1179,18 +1164,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>225</v>
-      </c>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1282,7 +1262,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B10" s="4" t="b">
         <v>0</v>
@@ -1294,10 +1274,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>232</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>237</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>1</v>
@@ -1424,7 +1404,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B22" s="7" t="b">
         <v>0</v>
@@ -1436,7 +1416,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B23" s="7" t="b">
         <v>0</v>
@@ -1550,7 +1530,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B32" s="7" t="b">
         <v>1</v>
@@ -1600,7 +1580,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B36" s="5" t="b">
         <v>1</v>
@@ -1681,10 +1661,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C43" s="12" t="s">
         <v>1</v>
@@ -1693,130 +1673,90 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>221</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>210</v>
       </c>
-      <c r="B44" s="11">
-        <v>50</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="B45" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="B46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="2"/>
+      <c r="B46">
+        <v>1920</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" s="2">
-        <v>100</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>7</v>
+      <c r="A47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>226</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>229</v>
+        <v>225</v>
+      </c>
+      <c r="B48">
+        <v>2018</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>213</v>
-      </c>
-      <c r="B49">
-        <v>1920</v>
+        <v>228</v>
+      </c>
+      <c r="B49" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" t="s">
-        <v>215</v>
+        <v>230</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B51">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>233</v>
-      </c>
-      <c r="B52" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>235</v>
-      </c>
-      <c r="B53">
-        <v>5</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>236</v>
-      </c>
-      <c r="B54">
-        <v>2010</v>
-      </c>
-      <c r="C54" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1836,7 +1776,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$1:$B$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B52 B35:B38 B8:B10 B14:B33</xm:sqref>
+          <xm:sqref>B49 B35:B38 B8:B10 B14:B33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -1860,13 +1800,13 @@
           <x14:formula1>
             <xm:f>dropdown!$I$9:$I$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B50</xm:sqref>
+          <xm:sqref>B47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>dropdown!$G$6:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B48</xm:sqref>
+          <xm:sqref>B45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1903,10 +1843,10 @@
         <v>194</v>
       </c>
       <c r="I1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1917,10 +1857,10 @@
         <v>195</v>
       </c>
       <c r="I2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1931,10 +1871,10 @@
         <v>192</v>
       </c>
       <c r="I3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1942,7 +1882,7 @@
         <v>190</v>
       </c>
       <c r="K4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1950,7 +1890,7 @@
         <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1958,7 +1898,7 @@
         <v>39</v>
       </c>
       <c r="G6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1966,7 +1906,7 @@
         <v>40</v>
       </c>
       <c r="G7" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1974,7 +1914,7 @@
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1982,7 +1922,7 @@
         <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1990,7 +1930,7 @@
         <v>43</v>
       </c>
       <c r="I10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1998,7 +1938,7 @@
         <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More cleaning of spreadsheets
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722BDA67-658F-4C4A-AD1D-B0802D88B560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B2C04C-A1C9-4FF5-89AB-3F3CC5B656F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1133,7 +1133,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1189,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1213,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1227,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Clean previous calibration targets and max prevalence
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP_TB_BMC_MED\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077B9C2D-7CBA-4AA6-82E1-CCFC20689AC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61BDEEC-912D-4D23-9452-573B9903253C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="241">
   <si>
     <t>project_name</t>
   </si>
@@ -661,9 +661,6 @@
     <t>find_a_calibrated_model</t>
   </si>
   <si>
-    <t>calibration_tolerance</t>
-  </si>
-  <si>
     <t>run_ks_based_calibration</t>
   </si>
   <si>
@@ -748,13 +745,10 @@
     <t>for SA</t>
   </si>
   <si>
-    <t>NOTV_lhs_50s_12r</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>alt_inf_analysis_50s_12r</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -1157,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,14 +1170,14 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1191,14 +1185,14 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1243,7 +1237,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1257,7 +1251,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
@@ -1292,10 +1286,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
@@ -1316,10 +1310,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="B12" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>1</v>
@@ -1331,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>1</v>
@@ -1574,7 +1565,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" s="7" t="b">
         <v>1</v>
@@ -1624,7 +1615,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B37" s="5" t="b">
         <v>1</v>
@@ -1705,10 +1696,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>1</v>
@@ -1717,109 +1708,106 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="B45" s="11">
-        <v>50</v>
+        <v>203</v>
+      </c>
+      <c r="B45" s="11" t="b">
+        <v>0</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>200</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B46" s="11" t="b">
+      <c r="A46" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B46" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="11"/>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" s="2" t="b">
-        <v>0</v>
+        <v>207</v>
+      </c>
+      <c r="B47" s="2">
+        <v>100</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B48" s="2">
-        <v>100</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>7</v>
+      <c r="A48" t="s">
+        <v>224</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>225</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>228</v>
+        <v>213</v>
+      </c>
+      <c r="B49">
+        <v>1920</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>214</v>
-      </c>
-      <c r="B50">
-        <v>1920</v>
+        <v>220</v>
+      </c>
+      <c r="B50" t="s">
+        <v>215</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" t="s">
-        <v>216</v>
+        <v>228</v>
+      </c>
+      <c r="B51">
+        <v>2018</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>229</v>
-      </c>
-      <c r="B52">
-        <v>2018</v>
+        <v>231</v>
+      </c>
+      <c r="B52" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>232</v>
-      </c>
-      <c r="B53" s="6" t="b">
-        <v>0</v>
+        <v>233</v>
+      </c>
+      <c r="B53">
+        <v>8</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1827,46 +1815,35 @@
         <v>234</v>
       </c>
       <c r="B54">
-        <v>8</v>
+        <v>2010</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>235</v>
       </c>
-      <c r="B55">
-        <v>2010</v>
+      <c r="B55" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B56" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C56" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D56" t="s">
         <v>238</v>
-      </c>
-      <c r="B57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1885,7 +1862,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$1:$B$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B53 B36:B39 B8:B11 B15:B34 B56:B57</xm:sqref>
+          <xm:sqref>B52 B36:B39 B8:B11 B15:B34 B55:B56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -1909,13 +1886,13 @@
           <x14:formula1>
             <xm:f>dropdown!$I$9:$I$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B51</xm:sqref>
+          <xm:sqref>B50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>dropdown!$G$6:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B49</xm:sqref>
+          <xm:sqref>B48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1952,10 +1929,10 @@
         <v>195</v>
       </c>
       <c r="I1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1966,7 +1943,7 @@
         <v>196</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K2" t="s">
         <v>210</v>
@@ -1980,10 +1957,10 @@
         <v>193</v>
       </c>
       <c r="I3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K3" t="s">
         <v>217</v>
-      </c>
-      <c r="K3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1991,7 +1968,7 @@
         <v>191</v>
       </c>
       <c r="K4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1999,7 +1976,7 @@
         <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2007,7 +1984,7 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2015,7 +1992,7 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2023,7 +2000,7 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2031,7 +2008,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2039,7 +2016,7 @@
         <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2047,7 +2024,7 @@
         <v>45</v>
       </c>
       <c r="I11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Import files from SNAP_TB_BMC_MED
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB_new\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP_TB_BMC_MED\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3AB737-1C51-498A-887D-5A3B6DABC7A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB3FA3F-16A6-4987-946B-9452D54A1FFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="242">
   <si>
     <t>project_name</t>
   </si>
@@ -661,6 +661,9 @@
     <t>find_a_calibrated_model</t>
   </si>
   <si>
+    <t>calibration_tolerance</t>
+  </si>
+  <si>
     <t>run_ks_based_calibration</t>
   </si>
   <si>
@@ -745,10 +748,7 @@
     <t>for SA</t>
   </si>
   <si>
-    <t>lhs_50s_12r</t>
-  </si>
-  <si>
-    <t>Bhutan/Mongolia/Viet Nam</t>
+    <t>NOTV_lhs_50s_12r</t>
   </si>
   <si>
     <t>200</t>
@@ -1154,10 +1154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,14 +1173,14 @@
         <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>240</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,14 +1188,14 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1204,7 +1204,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1216,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1254,7 +1254,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B10" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
@@ -1313,7 +1313,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B12" t="s">
+        <v>240</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>1</v>
@@ -1568,7 +1571,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B33" s="7" t="b">
         <v>1</v>
@@ -1618,7 +1621,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B37" s="5" t="b">
         <v>1</v>
@@ -1699,10 +1702,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>218</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>232</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>1</v>
@@ -1711,106 +1714,109 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B45" s="11">
+        <v>50</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="B45" s="11" t="b">
+      <c r="B46" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="11"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B46" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="2"/>
+      <c r="C46" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B48" s="2">
         <v>100</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>224</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>213</v>
-      </c>
-      <c r="B49">
-        <v>1920</v>
+        <v>225</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>228</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>220</v>
-      </c>
-      <c r="B50" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="B50">
+        <v>1920</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>228</v>
-      </c>
-      <c r="B51">
-        <v>2018</v>
+        <v>221</v>
+      </c>
+      <c r="B51" t="s">
+        <v>216</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>231</v>
-      </c>
-      <c r="B52" s="6" t="b">
-        <v>1</v>
+        <v>229</v>
+      </c>
+      <c r="B52">
+        <v>2018</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>233</v>
-      </c>
-      <c r="B53">
-        <v>50</v>
+        <v>232</v>
+      </c>
+      <c r="B53" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1818,35 +1824,46 @@
         <v>234</v>
       </c>
       <c r="B54">
-        <v>2010</v>
+        <v>8</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>235</v>
       </c>
-      <c r="B55" s="6" t="b">
-        <v>1</v>
+      <c r="B55">
+        <v>2010</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B56" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>238</v>
+      </c>
+      <c r="B57" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="C56" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D56" t="s">
-        <v>238</v>
+      <c r="C57" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1865,7 +1882,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$1:$B$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B52 B36:B39 B8:B11 B15:B34 B55:B56</xm:sqref>
+          <xm:sqref>B53 B36:B39 B8:B11 B15:B34 B56:B57</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -1889,13 +1906,13 @@
           <x14:formula1>
             <xm:f>dropdown!$I$9:$I$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B50</xm:sqref>
+          <xm:sqref>B51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>dropdown!$G$6:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B48</xm:sqref>
+          <xm:sqref>B49</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1932,10 +1949,10 @@
         <v>195</v>
       </c>
       <c r="I1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1946,7 +1963,7 @@
         <v>196</v>
       </c>
       <c r="I2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K2" t="s">
         <v>210</v>
@@ -1960,10 +1977,10 @@
         <v>193</v>
       </c>
       <c r="I3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1971,7 +1988,7 @@
         <v>191</v>
       </c>
       <c r="K4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1979,7 +1996,7 @@
         <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1987,7 +2004,7 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1995,7 +2012,7 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2003,7 +2020,7 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2011,7 +2028,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2019,7 +2036,7 @@
         <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2027,7 +2044,7 @@
         <v>45</v>
       </c>
       <c r="I11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Clean unused freezing demo variables
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rrag0004\Models\SNAP-TB\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEB0649-0D40-41E8-A88C-9399752E1E82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA931716-7914-474F-B945-C4ED0D9A43EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="239">
   <si>
     <t>project_name</t>
   </si>
@@ -644,12 +644,6 @@
   </si>
   <si>
     <t>/1000pop/y</t>
-  </si>
-  <si>
-    <t>freeze_demo</t>
-  </si>
-  <si>
-    <t>time_demo_freezing</t>
   </si>
   <si>
     <t>plot_ts_tb_prevalence_ds</t>
@@ -1151,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1171,7 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1185,14 +1179,14 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -1286,7 +1280,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B10" s="4" t="b">
         <v>0</v>
@@ -1310,7 +1304,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>1</v>
@@ -1437,7 +1431,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B23" s="7" t="b">
         <v>0</v>
@@ -1449,7 +1443,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B24" s="7" t="b">
         <v>0</v>
@@ -1563,7 +1557,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B33" s="7" t="b">
         <v>1</v>
@@ -1613,7 +1607,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B37" s="5" t="b">
         <v>1</v>
@@ -1694,10 +1688,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>1</v>
@@ -1706,7 +1700,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B45" s="11">
         <v>50</v>
@@ -1731,48 +1725,44 @@
       <c r="D46" s="11"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B47" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2"/>
+      <c r="A47" t="s">
+        <v>223</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B48" s="2">
-        <v>100</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48">
+        <v>1920</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>3</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>225</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>228</v>
+        <v>219</v>
+      </c>
+      <c r="B49" t="s">
+        <v>214</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="B50">
-        <v>1920</v>
+        <v>2020</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>3</v>
@@ -1780,21 +1770,21 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" t="s">
-        <v>216</v>
+        <v>230</v>
+      </c>
+      <c r="B51" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="B52">
-        <v>2020</v>
+        <v>8</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>3</v>
@@ -1802,60 +1792,38 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>232</v>
-      </c>
-      <c r="B53" s="6" t="b">
-        <v>1</v>
+        <v>233</v>
+      </c>
+      <c r="B53">
+        <v>2010</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>234</v>
       </c>
-      <c r="B54">
-        <v>8</v>
+      <c r="B54" s="6" t="b">
+        <v>1</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>235</v>
-      </c>
-      <c r="B55">
-        <v>2010</v>
+        <v>236</v>
+      </c>
+      <c r="B55" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>236</v>
-      </c>
-      <c r="B56" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>238</v>
-      </c>
-      <c r="B57" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
-        <v>239</v>
+        <v>10</v>
+      </c>
+      <c r="D55" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1874,7 +1842,7 @@
           <x14:formula1>
             <xm:f>dropdown!$A$1:$B$1</xm:f>
           </x14:formula1>
-          <xm:sqref>B53 B36:B39 B8:B11 B15:B34 B56:B57</xm:sqref>
+          <xm:sqref>B51 B36:B39 B8:B11 B15:B34 B54:B55</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -1898,13 +1866,13 @@
           <x14:formula1>
             <xm:f>dropdown!$I$9:$I$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B51</xm:sqref>
+          <xm:sqref>B49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>dropdown!$G$6:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B49</xm:sqref>
+          <xm:sqref>B47</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1941,10 +1909,10 @@
         <v>195</v>
       </c>
       <c r="I1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1955,10 +1923,10 @@
         <v>196</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1969,10 +1937,10 @@
         <v>193</v>
       </c>
       <c r="I3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1980,7 +1948,7 @@
         <v>191</v>
       </c>
       <c r="K4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1988,7 +1956,7 @@
         <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1996,7 +1964,7 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2004,7 +1972,7 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2012,7 +1980,7 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2020,7 +1988,7 @@
         <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2028,7 +1996,7 @@
         <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2036,7 +2004,7 @@
         <v>45</v>
       </c>
       <c r="I11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>